<commit_message>
finish data loader and updated coffee_shop_images
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/Menu_coffeeShop.xlsx
+++ b/src/main/resources/assets/Menu_coffeeShop.xlsx
@@ -83,7 +83,7 @@
     <t>Iced Mocha</t>
   </si>
   <si>
-    <t>Espresso, chocolate, milk, and ice.</t>
+    <t>Muff</t>
   </si>
   <si>
     <t>Iced Coffee</t>
@@ -169,7 +169,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +185,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="19"/>
       <color rgb="FF262626"/>
@@ -193,7 +199,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -244,57 +250,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,7 +623,7 @@
     <col min="1" max="1" style="14" width="2.5764285714285715" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="15" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="16" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="29.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -637,7 +640,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A3" s="4"/>
       <c r="B3" s="7" t="s">
         <v>1</v>
@@ -657,7 +660,7 @@
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A5" s="4"/>
       <c r="B5" s="10" t="s">
         <v>5</v>
@@ -669,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A6" s="4"/>
       <c r="B6" s="10" t="s">
         <v>7</v>
@@ -681,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="28.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A7" s="4"/>
       <c r="B7" s="10" t="s">
         <v>9</v>
@@ -693,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="28.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
         <v>11</v>
@@ -705,7 +708,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="28.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A9" s="4"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -717,7 +720,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="28.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A10" s="4"/>
       <c r="B10" s="10" t="s">
         <v>15</v>
@@ -743,7 +746,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="28.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A13" s="4"/>
       <c r="B13" s="10" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
added products to DatabaseLoader
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/Menu_coffeeShop.xlsx
+++ b/src/main/resources/assets/Menu_coffeeShop.xlsx
@@ -178,6 +178,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color rgb="FF1c639e"/>
@@ -186,7 +192,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -195,12 +201,6 @@
       <sz val="19"/>
       <color rgb="FF262626"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -250,30 +250,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
@@ -282,9 +279,6 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -292,13 +286,13 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="7" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,10 +614,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="2.5764285714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="15" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="2.5764285714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="29.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
@@ -642,19 +636,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A4" s="4"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3"/>
@@ -662,85 +656,85 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A5" s="4"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A6" s="4"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="3">
         <v>4.5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A7" s="4"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="3">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A8" s="4"/>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A9" s="4"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="3">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A10" s="4"/>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A11" s="4"/>
-      <c r="B11" s="12"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A12" s="4"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="3"/>
@@ -748,135 +742,135 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33" customFormat="1" s="6">
       <c r="A13" s="4"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="3">
         <v>5</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="28.5" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A14" s="4"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="3">
         <v>6</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A15" s="4"/>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="3">
         <v>4</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="30" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="33.75" customFormat="1" s="6">
       <c r="A16" s="4"/>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="3">
         <v>6</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="30" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="33.75" customFormat="1" s="6">
       <c r="A17" s="4"/>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="3">
         <v>4.5</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="30" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A18" s="4"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="30" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A19" s="4"/>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="30" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A20" s="4"/>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="3">
         <v>3.5</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="30" customFormat="1" s="6">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A21" s="4"/>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="3">
         <v>3.5</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A22" s="4"/>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="3">
         <v>3.5</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A23" s="4"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="3">
         <v>3.5</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A24" s="4"/>
-      <c r="B24" s="12"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A25" s="4"/>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="3"/>
@@ -884,55 +878,55 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A26" s="4"/>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="3">
         <v>3</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A27" s="4"/>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="3">
         <v>3</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A28" s="4"/>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="3">
         <v>1.5</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A29" s="4"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="11"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A30" s="4"/>
-      <c r="B30" s="12"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A31" s="4"/>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C31" s="3"/>
@@ -940,109 +934,109 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A32" s="4"/>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="3">
         <v>1</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A33" s="4"/>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="3">
         <v>2.99</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A34" s="4"/>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="3">
         <v>1</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A35" s="4"/>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="3">
         <v>1</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A36" s="4"/>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="3">
         <v>1</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A37" s="4"/>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="3">
         <v>1</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A38" s="4"/>
-      <c r="B38" s="12"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A39" s="4"/>
-      <c r="B39" s="12"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="3"/>
       <c r="D39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A40" s="4"/>
-      <c r="B40" s="12"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="3"/>
       <c r="D40" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A41" s="4"/>
-      <c r="B41" s="12"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A42" s="4"/>
-      <c r="B42" s="12"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A43" s="4"/>
-      <c r="B43" s="12"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="3"/>
       <c r="D43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A44" s="4"/>
-      <c r="B44" s="12"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="3"/>
       <c r="D44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="30" customFormat="1" s="6">
       <c r="A45" s="4"/>
-      <c r="B45" s="12"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="3"/>
       <c r="D45" s="4"/>
     </row>

</xml_diff>